<commit_message>
Calibration of bldgs and transp
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Virginia\VA_Model\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Nevada\NV_model\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F426623E-986B-4896-AF4D-49046E042502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD81673-2C12-4BBA-AA42-12BCD2035B8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="1920" windowWidth="9930" windowHeight="13770" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="11430" windowHeight="13575" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26384,7 +26384,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26414,13 +26414,13 @@
         <v>3</v>
       </c>
       <c r="B2">
+        <v>5.2080000000000001E-2</v>
+      </c>
+      <c r="C2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="C2">
-        <v>4.5999999999999999E-2</v>
-      </c>
       <c r="D2">
-        <v>6.4399999999999999E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26428,10 +26428,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>6.4799999999999996E-2</v>
+        <v>6.2199999999999998E-2</v>
       </c>
       <c r="C3">
-        <v>6.25E-2</v>
+        <v>6.2199999999999998E-2</v>
       </c>
       <c r="D3">
         <v>6.2199999999999998E-2</v>
@@ -26456,13 +26456,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.13</v>
+        <v>0.11749999999999999</v>
       </c>
       <c r="C5">
-        <v>0.13</v>
+        <v>0.11905</v>
       </c>
       <c r="D5">
-        <v>0.11</v>
+        <v>0.1105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>